<commit_message>
Add ccoment in ST
</commit_message>
<xml_diff>
--- a/Listado COMVEN LID AFIP.xlsx
+++ b/Listado COMVEN LID AFIP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos Uipath\Descarga-y-Carga-COMVEN-LID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69429415-6B11-4F6D-AA52-82DFCC99E375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE216FA-1BAB-4FB4-9F01-5AA04ABF6E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,6 +91,30 @@
           </rPr>
           <t xml:space="preserve">
 CUIT del representado </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{87C20348-1149-4E0A-8D41-CA0F1FD6254E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Agustín Bustos:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Si el archivo no se guarda con el nombre a medida se debe colocar "NO" en esta columna </t>
         </r>
       </text>
     </comment>
@@ -2000,7 +2024,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>